<commit_message>
Experiment 3 and Statistical Analysis
</commit_message>
<xml_diff>
--- a/Trials n=12(AutoRecovered).xlsx
+++ b/Trials n=12(AutoRecovered).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shevyapanda/Desktop/personalprojects/PALS_Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91895A32-E3DE-1C4B-836F-A1CD5411FD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4673A9EE-6197-E14F-9EFC-96E33CF09CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="64">
   <si>
     <t>Patient ID</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Average Paramater Score</t>
+  </si>
+  <si>
+    <t>see exp 3 analysis</t>
   </si>
 </sst>
 </file>
@@ -6100,8 +6103,8 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:I41"/>
+    <sheetView zoomScale="61" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7409,10 +7412,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CD6663-3B07-214D-ADED-F9743E2B2B70}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7438,6 +7441,11 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B4" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:Q1"/>

</xml_diff>